<commit_message>
20251204 Small / Small Midcaps updated + Elux
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202509/DEUPT.xlsx
+++ b/GUI + Reviews/202509/DEUPT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\PM-Indices-IndexOperations\Review Files\202509\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/202509/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29523660-3AF3-4C24-BF1B-24BFF63DB5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{29523660-3AF3-4C24-BF1B-24BFF63DB5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83ACB09A-A7B7-41C5-82A0-3BFFF9868F67}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C6008D35-8125-4B38-A978-A72297B582E2}"/>
+    <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15720" xr2:uid="{C6008D35-8125-4B38-A978-A72297B582E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12107,22 +12107,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1AAFA654-6B1F-42CE-9433-BD6A41127AE0}" name="Universe" displayName="Universe" ref="A1:M1295" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1AAFA654-6B1F-42CE-9433-BD6A41127AE0}" name="Universe" displayName="Universe" ref="A1:M1295" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:M1295" xr:uid="{1AAFA654-6B1F-42CE-9433-BD6A41127AE0}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{6C097E18-57B2-4056-BCB6-4621EC19FB3B}" name="Name" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{6C90EBE1-AABA-4567-9CF8-C2AE7E4B6CBC}" name="Ticker" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{A7D3FA48-24AB-45D8-BF97-EDF876C9907D}" name="ISIN" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{44C55F4F-E74C-4D5C-A2B9-1D86A3B0221C}" name="MIC" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{EFBEBDBE-2766-485C-B918-9D88ABC09B69}" name="Currency (Local)" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{3AD75462-29CB-426C-AA24-94FC3EA949BF}" name="Price (EUR) " dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{711D9367-C299-4D74-B464-CEF998D02332}" name="NOSH" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{280E286A-E940-41EF-A56A-712AF6E7A9F8}" name="20 days AVG turnover EUR" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{197B4ACF-6025-4693-8297-2FE32DBA4EBA}" name="3M AVG Turnover EUR" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{C7328995-4909-4577-8E15-F688D3FDE76C}" name="3M AVG Turnover USD" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{F639C653-BE4A-42BD-B4A9-59014677E54A}" name="100 Trading Days AVG Turnover EUR" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{E7A36952-FD0D-4165-BEC2-31EAFCEDDF9E}" name="6M AVG Turnover EUR" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{4B07B0CC-2AB2-468A-8966-BA3F04FEF88A}" name="12M AVG Turnover EUR" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{6C097E18-57B2-4056-BCB6-4621EC19FB3B}" name="Name" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{6C90EBE1-AABA-4567-9CF8-C2AE7E4B6CBC}" name="Ticker" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{A7D3FA48-24AB-45D8-BF97-EDF876C9907D}" name="ISIN" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{44C55F4F-E74C-4D5C-A2B9-1D86A3B0221C}" name="MIC" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{EFBEBDBE-2766-485C-B918-9D88ABC09B69}" name="Currency (Local)" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{3AD75462-29CB-426C-AA24-94FC3EA949BF}" name="Price (EUR) " dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{711D9367-C299-4D74-B464-CEF998D02332}" name="NOSH" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{280E286A-E940-41EF-A56A-712AF6E7A9F8}" name="20 days AVG turnover EUR" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{197B4ACF-6025-4693-8297-2FE32DBA4EBA}" name="3M AVG Turnover EUR" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{C7328995-4909-4577-8E15-F688D3FDE76C}" name="3M AVG Turnover USD" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{F639C653-BE4A-42BD-B4A9-59014677E54A}" name="100 Trading Days AVG Turnover EUR" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{E7A36952-FD0D-4165-BEC2-31EAFCEDDF9E}" name="6M AVG Turnover EUR" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{4B07B0CC-2AB2-468A-8966-BA3F04FEF88A}" name="12M AVG Turnover EUR" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12447,7 +12447,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE6A6399-A6B1-4482-BD77-BA00E1F17332}">
   <dimension ref="A1:M1295"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:P22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>